<commit_message>
cigna changes in progress
</commit_message>
<xml_diff>
--- a/Input/Cigna_Global_Health/cignaScript/inputRates/benefits.xlsx
+++ b/Input/Cigna_Global_Health/cignaScript/inputRates/benefits.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="168">
   <si>
     <t xml:space="preserve">PlanName</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t xml:space="preserve">addons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$copay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$outPatient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$vaccination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$physiotherepy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$medicines</t>
   </si>
   <si>
     <t xml:space="preserve">Platinum</t>
@@ -200,21 +215,21 @@
     <t xml:space="preserve">Private room</t>
   </si>
   <si>
+    <t xml:space="preserve">Covered up to USD 14,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 months wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered up to USD 28,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered up to USD 156,000 for 90 days</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optional Benefit</t>
   </si>
   <si>
-    <t xml:space="preserve">Covered up to USD 14,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 months wait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to USD 28,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covered up to USD 156,000 for 90 days</t>
-  </si>
-  <si>
     <t xml:space="preserve">Acupuncture and Chinese medicine covered in full</t>
   </si>
   <si>
@@ -252,6 +267,21 @@
   </si>
   <si>
     <t xml:space="preserve">Worldwide including USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered up to USD 2,500 - $0, 0% Co-insurance/$0, 10% Co-insurance, $3,000 Out of pocket/$0, 20% Co-insurance, $3,000 Out of pocket/$0, 30% Co-insurance, $3,000 Out of pocket/$1,000, 0% Co-insurance/$1,000, 10% Co-insurance, $3,000 Out of pocket/$1,000, 20% Co-insurance, $3,000 Out of pocket/$1,000, 30% Co-insurance, $3,000 Out of pocket/$1,500, 0% Co-insurance$1,500, 10% Co-insurance, $3,000 Out of pocket/$1,500, 20% Co-insurance, $3,000 Out of pocket/$1,500, 30% Co-insurance, $3,000 Out of pocket/$150, 0% Co-insurance/$150, 10% Co-insurance, $3,000 Out of pocket/$150, 20% Co-insurance, $3,000 Out of pocket/$150, 30% Co-insurance, $3,000 Out of pocket/$500, 0% Co-insurance/$500, 10% Co-insurance, $3,000 Out of pocket/$500, 20% Co-insurance, $3,000 Out of pocket/$500, 30% Co-insurance, $3,000 Out of pocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicines covered up to USD 1,500, Diagnostics &amp; lab tests covered up to USD 2,500  Consultation covered up to USD 2,500 - $0, 0% Co-insurance/$0, 10% Co-insurance, $3,000 Out of pocket/$0, 20% Co-insurance, $3,000 Out of pocket/$0, 30% Co-insurance, $3,000 Out of pocket/$1,000, 0% Co-insurance/$1,000, 10% Co-insurance, $3,000 Out of pocket/$1,000, 20% Co-insurance, $3,000 Out of pocket/$1,000, 30% Co-insurance, $3,000 Out of pocket/$1,500, 0% Co-insurance$1,500, 10% Co-insurance, $3,000 Out of pocket/$1,500, 20% Co-insurance, $3,000 Out of pocket/$1,500, 30% Co-insurance, $3,000 Out of pocket/$150, 0% Co-insurance/$150, 10% Co-insurance, $3,000 Out of pocket/$150, 20% Co-insurance, $3,000 Out of pocket/$150, 30% Co-insurance, $3,000 Out of pocket/$500, 0% Co-insurance/$500, 10% Co-insurance, $3,000 Out of pocket/$500, 20% Co-insurance, $3,000 Out of pocket/$500, 30% Co-insurance, $3,000 Out of pocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adults- Covered up to USD 250 - $0, 0% Co-insurance/$0, 10% Co-insurance, $3,000 Out of pocket/$0, 20% Co-insurance, $3,000 Out of pocket/$0, 30% Co-insurance, $3,000 Out of pocket/$1,000, 0% Co-insurance/$1,000, 10% Co-insurance, $3,000 Out of pocket/$1,000, 20% Co-insurance, $3,000 Out of pocket/$1,000, 30% Co-insurance, $3,000 Out of pocket/$1,500, 0% Co-insurance$1,500, 10% Co-insurance, $3,000 Out of pocket/$1,500, 20% Co-insurance, $3,000 Out of pocket/$1,500, 30% Co-insurance, $3,000 Out of pocket/$150, 0% Co-insurance/$150, 10% Co-insurance, $3,000 Out of pocket/$150, 20% Co-insurance, $3,000 Out of pocket/$150, 30% Co-insurance, $3,000 Out of pocket/$500, 0% Co-insurance/$500, 10% Co-insurance, $3,000 Out of pocket/$500, 20% Co-insurance, $3,000 Out of pocket/$500, 30% Co-insurance, $3,000 Out of pocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered up to USD 5,000 (Combined benefit) - $0, 0% Co-insurance/$0, 10% Co-insurance, $3,000 Out of pocket/$0, 20% Co-insurance, $3,000 Out of pocket/$0, 30% Co-insurance, $3,000 Out of pocket/$1,000, 0% Co-insurance/$1,000, 10% Co-insurance, $3,000 Out of pocket/$1,000, 20% Co-insurance, $3,000 Out of pocket/$1,000, 30% Co-insurance, $3,000 Out of pocket/$1,500, 0% Co-insurance$1,500, 10% Co-insurance, $3,000 Out of pocket/$1,500, 20% Co-insurance, $3,000 Out of pocket/$1,500, 30% Co-insurance, $3,000 Out of pocket/$150, 0% Co-insurance/$150, 10% Co-insurance, $3,000 Out of pocket/$150, 20% Co-insurance, $3,000 Out of pocket/$150, 30% Co-insurance, $3,000 Out of pocket/$500, 0% Co-insurance/$500, 10% Co-insurance, $3,000 Out of pocket/$500, 20% Co-insurance, $3,000 Out of pocket/$500, 30% Co-insurance, $3,000 Out of pocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covered up to USD 1,500 - $0, 0% Co-insurance/$0, 10% Co-insurance, $3,000 Out of pocket/$0, 20% Co-insurance, $3,000 Out of pocket/$0, 30% Co-insurance, $3,000 Out of pocket/$1,000, 0% Co-insurance/$1,000, 10% Co-insurance, $3,000 Out of pocket/$1,000, 20% Co-insurance, $3,000 Out of pocket/$1,000, 30% Co-insurance, $3,000 Out of pocket/$1,500, 0% Co-insurance$1,500, 10% Co-insurance, $3,000 Out of pocket/$1,500, 20% Co-insurance, $3,000 Out of pocket/$1,500, 30% Co-insurance, $3,000 Out of pocket/$150, 0% Co-insurance/$150, 10% Co-insurance, $3,000 Out of pocket/$150, 20% Co-insurance, $3,000 Out of pocket/$150, 30% Co-insurance, $3,000 Out of pocket/$500, 0% Co-insurance/$500, 10% Co-insurance, $3,000 Out of pocket/$500, 20% Co-insurance, $3,000 Out of pocket/$500, 30% Co-insurance, $3,000 Out of pocket</t>
   </si>
   <si>
     <t xml:space="preserve">Silver</t>
@@ -505,7 +535,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -532,6 +562,17 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,13 +617,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -605,8 +650,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -626,13 +679,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BA50"/>
+  <dimension ref="A1:BF50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AQ1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AU4" activeCellId="0" sqref="AU4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BD1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BE2" activeCellId="0" sqref="BE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="11.52"/>
@@ -641,144 +694,149 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="36.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="41.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="2" width="37.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="2" width="44.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="2" width="51.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="2" width="61.69"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="2" t="s">
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AN1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="2" t="s">
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AR1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AS1" s="3" t="s">
         <v>42</v>
       </c>
       <c r="AT1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="6" t="s">
+      <c r="AU1" s="7" t="s">
         <v>44</v>
       </c>
       <c r="AV1" s="0" t="s">
@@ -799,715 +857,749 @@
       <c r="BA1" s="0" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="57.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="BC1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="BD1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="2" t="s">
+      <c r="BF1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="269.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="5"/>
+      <c r="W2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU2" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BA2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB2" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="BF2" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="2" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS2" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT2" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AU2" s="0" t="s">
+      <c r="J3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" s="5"/>
+      <c r="W3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AV2" s="0" t="s">
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AR3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AX2" s="7" t="s">
+      <c r="AS3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AY2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BA2" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="V3" s="4"/>
-      <c r="W3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO3" s="4"/>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR3" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT3" s="6" t="s">
-        <v>83</v>
+      <c r="AT3" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="AU3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AZ3" s="4" t="s">
-        <v>85</v>
+        <v>94</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="BA3" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="2" t="s">
+    <row r="4" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4" s="4"/>
-      <c r="W4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="X4" s="2" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Y4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR4" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT4" s="6" t="s">
-        <v>93</v>
+      <c r="H4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V4" s="5"/>
+      <c r="W4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT4" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="AU4" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="BA4" s="0" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT5" s="6" t="s">
-        <v>95</v>
+      <c r="AT5" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="AU5" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="BA5" s="0" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT6" s="6" t="s">
-        <v>97</v>
+      <c r="O6" s="2"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="2"/>
+      <c r="AT6" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="AU6" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="BA6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="BA6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT7" s="6" t="s">
-        <v>99</v>
+      <c r="AT7" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="AU7" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="BA7" s="0" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT8" s="6" t="s">
-        <v>101</v>
+      <c r="AT8" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="AU8" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="BA8" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT9" s="6" t="s">
-        <v>103</v>
+      <c r="AT9" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="AU9" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="BA9" s="0" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT10" s="6" t="s">
-        <v>105</v>
+      <c r="AT10" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="AU10" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="BA10" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT11" s="6" t="s">
-        <v>107</v>
+      <c r="AT11" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="AU11" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="BA11" s="0" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT12" s="6" t="s">
-        <v>109</v>
+      <c r="AT12" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="AU12" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="BA12" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT13" s="6" t="s">
-        <v>111</v>
+      <c r="AT13" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="AU13" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="BA13" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT14" s="6" t="s">
-        <v>113</v>
+      <c r="AT14" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="AU14" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT15" s="6" t="s">
-        <v>115</v>
+      <c r="AT15" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="AU15" s="0" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT16" s="6" t="s">
-        <v>117</v>
+      <c r="AT16" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="AU16" s="0" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT17" s="6" t="s">
-        <v>119</v>
+      <c r="AT17" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="AU17" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT18" s="6" t="s">
-        <v>121</v>
+      <c r="AT18" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="AU18" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT19" s="6" t="s">
-        <v>123</v>
+      <c r="AT19" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="AU19" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT20" s="6" t="s">
-        <v>125</v>
+      <c r="AT20" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="AU20" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT21" s="6" t="s">
-        <v>127</v>
+      <c r="AT21" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="AU21" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT22" s="6" t="s">
-        <v>129</v>
+      <c r="AT22" s="7" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT23" s="6" t="s">
-        <v>130</v>
+      <c r="AT23" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT24" s="6" t="s">
-        <v>131</v>
+      <c r="AT24" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT25" s="6" t="s">
-        <v>132</v>
+      <c r="AT25" s="7" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT26" s="6" t="s">
-        <v>133</v>
+      <c r="AT26" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT27" s="6" t="s">
-        <v>134</v>
+      <c r="AT27" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT28" s="6" t="s">
-        <v>135</v>
+      <c r="AT28" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT29" s="6" t="s">
-        <v>136</v>
+      <c r="AT29" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT30" s="6" t="s">
-        <v>137</v>
+      <c r="AT30" s="7" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT31" s="6" t="s">
-        <v>138</v>
+      <c r="AT31" s="7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT32" s="6" t="s">
-        <v>139</v>
+      <c r="AT32" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT33" s="6" t="s">
-        <v>140</v>
+      <c r="AT33" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT34" s="6" t="s">
-        <v>141</v>
+      <c r="AT34" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT35" s="6" t="s">
-        <v>142</v>
+      <c r="AT35" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT36" s="6" t="s">
-        <v>143</v>
+      <c r="AT36" s="7" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT37" s="6" t="s">
-        <v>144</v>
+      <c r="AT37" s="7" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT38" s="6" t="s">
-        <v>145</v>
+      <c r="AT38" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT39" s="6" t="s">
-        <v>146</v>
+      <c r="AT39" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT40" s="6" t="s">
-        <v>147</v>
+      <c r="AT40" s="7" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT41" s="6" t="s">
-        <v>148</v>
+      <c r="AT41" s="7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT42" s="6" t="s">
-        <v>149</v>
+      <c r="AT42" s="7" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT43" s="6" t="s">
-        <v>150</v>
+      <c r="AT43" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT44" s="6" t="s">
-        <v>151</v>
+      <c r="AT44" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT45" s="6" t="s">
-        <v>152</v>
+      <c r="AT45" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT46" s="6" t="s">
-        <v>153</v>
+      <c r="AT46" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT47" s="6" t="s">
-        <v>154</v>
+      <c r="AT47" s="7" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT48" s="6" t="s">
-        <v>155</v>
+      <c r="AT48" s="7" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT49" s="6" t="s">
-        <v>156</v>
+      <c r="AT49" s="7" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AT50" s="6" t="s">
-        <v>157</v>
+      <c r="AT50" s="7" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>